<commit_message>
tool script creater after test create script package for 02 gnodeb
test successful create 02 script package at a sametime
</commit_message>
<xml_diff>
--- a/script_creater/input_cdd.xlsx
+++ b/script_creater/input_cdd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin\home\ephucle\tool_script\python\pythonlab\script_creater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06939542-55AA-4C3C-AABD-CCA5FD025B4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A3F2F0-DFAC-47F1-A7D3-0ECBAF46B785}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" activeTab="1" xr2:uid="{C5C6894B-A5F7-4A64-8BB5-8FA162EF2999}"/>
   </bookViews>
@@ -908,6 +908,17 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="4.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>